<commit_message>
customized updated mexico files bceu, drc, bnvfe, bhnvfe, syfafe, bifubc
</commit_message>
<xml_diff>
--- a/InputData/bldgs/BCEU/BAU Components Energy Use.xlsx
+++ b/InputData/bldgs/BCEU/BAU Components Energy Use.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anaxolt/Google Drive/2021/D.Development/TARGET_eps-us-3.2.1/InputData/bldgs/BCEU/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B965527F-5215-2C47-8FE7-58BA097CE72E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D07E02E-663E-F840-8024-93C8E2CB6648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3940" yWindow="-21100" windowWidth="34440" windowHeight="20040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -1696,17 +1696,17 @@
     <xf numFmtId="0" fontId="39" fillId="6" borderId="0" xfId="20" applyFont="1" applyFill="1"/>
     <xf numFmtId="170" fontId="40" fillId="6" borderId="0" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="170" fontId="41" fillId="6" borderId="0" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="22">
     <cellStyle name="Body: normal cell" xfId="4" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -9222,8 +9222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9535,7 +9535,7 @@
   <dimension ref="A1:AI36"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:AG11"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9921,131 +9921,131 @@
       </c>
       <c r="B4" s="7">
         <f>BCEU_consumoBTU!D7*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>21175510062860.918</v>
+        <v>1270530603771.655</v>
       </c>
       <c r="C4" s="7">
         <f>BCEU_consumoBTU!E7*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>21263412981816.402</v>
+        <v>1275804778908.9841</v>
       </c>
       <c r="D4" s="7">
         <f>BCEU_consumoBTU!F7*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>21360409306181.066</v>
+        <v>1281624558370.864</v>
       </c>
       <c r="E4" s="7">
         <f>BCEU_consumoBTU!G7*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>21433156549454.566</v>
+        <v>1285989392967.2739</v>
       </c>
       <c r="F4" s="7">
         <f>BCEU_consumoBTU!H7*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>21484685846773.297</v>
+        <v>1289081150806.3977</v>
       </c>
       <c r="G4" s="7">
         <f>BCEU_consumoBTU!I7*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>21545308549501.207</v>
+        <v>1292718512970.0723</v>
       </c>
       <c r="H4" s="7">
         <f>BCEU_consumoBTU!J7*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>21596837846819.934</v>
+        <v>1295810270809.196</v>
       </c>
       <c r="I4" s="7">
         <f>BCEU_consumoBTU!K7*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>21657460549547.852</v>
+        <v>1299447632972.8711</v>
       </c>
       <c r="J4" s="7">
         <f>BCEU_consumoBTU!L7*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>21715052117139.371</v>
+        <v>1302903127028.3623</v>
       </c>
       <c r="K4" s="7">
         <f>BCEU_consumoBTU!M7*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>21775674819867.289</v>
+        <v>1306540489192.0374</v>
       </c>
       <c r="L4" s="7">
         <f>BCEU_consumoBTU!N7*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>21833266387458.801</v>
+        <v>1309995983247.5281</v>
       </c>
       <c r="M4" s="7">
         <f>BCEU_consumoBTU!O7*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>21890857955050.328</v>
+        <v>1313451477303.0195</v>
       </c>
       <c r="N4" s="7">
         <f>BCEU_consumoBTU!P7*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>21884795684777.539</v>
+        <v>1313087741086.6523</v>
       </c>
       <c r="O4" s="7">
         <f>BCEU_consumoBTU!Q7*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>22213067620049.195</v>
+        <v>1332784057202.9517</v>
       </c>
       <c r="P4" s="7">
         <f>BCEU_consumoBTU!R7*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>22546263634349.93</v>
+        <v>1352775818060.9958</v>
       </c>
       <c r="Q4" s="7">
         <f>BCEU_consumoBTU!S7*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>22884457588865.18</v>
+        <v>1373067455331.9106</v>
       </c>
       <c r="R4" s="7">
         <f>BCEU_consumoBTU!T7*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>23227724452698.156</v>
+        <v>1393663467161.8894</v>
       </c>
       <c r="S4" s="7">
         <f>BCEU_consumoBTU!U7*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>23576140319488.625</v>
+        <v>1414568419169.3174</v>
       </c>
       <c r="T4" s="7">
         <f>BCEU_consumoBTU!V7*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>23929782424280.949</v>
+        <v>1435786945456.8569</v>
       </c>
       <c r="U4" s="7">
         <f>BCEU_consumoBTU!W7*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>24288729160645.168</v>
+        <v>1457323749638.71</v>
       </c>
       <c r="V4" s="7">
         <f>BCEU_consumoBTU!X7*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>24653060098054.84</v>
+        <v>1479183605883.2903</v>
       </c>
       <c r="W4" s="7">
         <f>BCEU_consumoBTU!Y7*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>25022855999525.66</v>
+        <v>1501371359971.5396</v>
       </c>
       <c r="X4" s="7">
         <f>BCEU_consumoBTU!Z7*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>25398198839518.543</v>
+        <v>1523891930371.1125</v>
       </c>
       <c r="Y4" s="7">
         <f>BCEU_consumoBTU!AA7*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>25779171822111.32</v>
+        <v>1546750309326.6792</v>
       </c>
       <c r="Z4" s="7">
         <f>BCEU_consumoBTU!AB7*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>26165859399442.988</v>
+        <v>1569951563966.5793</v>
       </c>
       <c r="AA4" s="7">
         <f>BCEU_consumoBTU!AC7*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>26558347290434.633</v>
+        <v>1593500837426.0779</v>
       </c>
       <c r="AB4" s="7">
         <f>BCEU_consumoBTU!AD7*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>26956722499791.148</v>
+        <v>1617403349987.4688</v>
       </c>
       <c r="AC4" s="7">
         <f>BCEU_consumoBTU!AE7*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>27361073337288.012</v>
+        <v>1641664400237.2808</v>
       </c>
       <c r="AD4" s="7">
         <f>BCEU_consumoBTU!AF7*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>27771489437347.328</v>
+        <v>1666289366240.8396</v>
       </c>
       <c r="AE4" s="7">
         <f>BCEU_consumoBTU!AG7*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>28188061778907.535</v>
+        <v>1691283706734.4521</v>
       </c>
       <c r="AF4" s="7">
         <f>BCEU_consumoBTU!AH7*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>28610882705591.145</v>
+        <v>1716652962335.4685</v>
       </c>
       <c r="AG4" s="7">
         <f>BCEU_consumoBTU!AI7*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>29040045946175.016</v>
+        <v>1742402756770.501</v>
       </c>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.2">
@@ -10320,131 +10320,131 @@
       </c>
       <c r="B7" s="7">
         <f>BCEU_consumoBTU!D10*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>175344398105357.91</v>
+        <v>0</v>
       </c>
       <c r="C7" s="7">
         <f>BCEU_consumoBTU!E10*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>172502311314361.97</v>
+        <v>0</v>
       </c>
       <c r="D7" s="7">
         <f>BCEU_consumoBTU!F10*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>170731155777944.22</v>
+        <v>0</v>
       </c>
       <c r="E7" s="7">
         <f>BCEU_consumoBTU!G10*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>168095017305136.41</v>
+        <v>0</v>
       </c>
       <c r="F7" s="7">
         <f>BCEU_consumoBTU!H10*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>165953154795980.03</v>
+        <v>0</v>
       </c>
       <c r="G7" s="7">
         <f>BCEU_consumoBTU!I10*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>163111068004984.09</v>
+        <v>0</v>
       </c>
       <c r="H7" s="7">
         <f>BCEU_consumoBTU!J10*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>161339912468566.34</v>
+        <v>0</v>
       </c>
       <c r="I7" s="7">
         <f>BCEU_consumoBTU!K10*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>158992101641221.88</v>
+        <v>0</v>
       </c>
       <c r="J7" s="7">
         <f>BCEU_consumoBTU!L10*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>156809049468427.91</v>
+        <v>0</v>
       </c>
       <c r="K7" s="7">
         <f>BCEU_consumoBTU!M10*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>154131721331982.47</v>
+        <v>0</v>
       </c>
       <c r="L7" s="7">
         <f>BCEU_consumoBTU!N10*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>152566514113752.81</v>
+        <v>0</v>
       </c>
       <c r="M7" s="7">
         <f>BCEU_consumoBTU!O10*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>149600858331844</v>
+        <v>0</v>
       </c>
       <c r="N7" s="7">
         <f>BCEU_consumoBTU!P10*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>147582564813600.5</v>
+        <v>0</v>
       </c>
       <c r="O7" s="7">
         <f>BCEU_consumoBTU!Q10*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>146844651989532.53</v>
+        <v>0</v>
       </c>
       <c r="P7" s="7">
         <f>BCEU_consumoBTU!R10*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>146110428729584.88</v>
+        <v>0</v>
       </c>
       <c r="Q7" s="7">
         <f>BCEU_consumoBTU!S10*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>145379876585936.97</v>
+        <v>0</v>
       </c>
       <c r="R7" s="7">
         <f>BCEU_consumoBTU!T10*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>144652977203007.25</v>
+        <v>0</v>
       </c>
       <c r="S7" s="7">
         <f>BCEU_consumoBTU!U10*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>143929712316992.22</v>
+        <v>0</v>
       </c>
       <c r="T7" s="7">
         <f>BCEU_consumoBTU!V10*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>143210063755407.25</v>
+        <v>0</v>
       </c>
       <c r="U7" s="7">
         <f>BCEU_consumoBTU!W10*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>142494013436630.22</v>
+        <v>0</v>
       </c>
       <c r="V7" s="7">
         <f>BCEU_consumoBTU!X10*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>141781543369447.06</v>
+        <v>0</v>
       </c>
       <c r="W7" s="7">
         <f>BCEU_consumoBTU!Y10*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>141072635652599.84</v>
+        <v>0</v>
       </c>
       <c r="X7" s="7">
         <f>BCEU_consumoBTU!Z10*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>140367272474336.83</v>
+        <v>0</v>
       </c>
       <c r="Y7" s="7">
         <f>BCEU_consumoBTU!AA10*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>139665436111965.16</v>
+        <v>0</v>
       </c>
       <c r="Z7" s="7">
         <f>BCEU_consumoBTU!AB10*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>138967108931405.34</v>
+        <v>0</v>
       </c>
       <c r="AA7" s="7">
         <f>BCEU_consumoBTU!AC10*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>138272273386748.3</v>
+        <v>0</v>
       </c>
       <c r="AB7" s="7">
         <f>BCEU_consumoBTU!AD10*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>137580912019814.53</v>
+        <v>0</v>
       </c>
       <c r="AC7" s="7">
         <f>BCEU_consumoBTU!AE10*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>136893007459715.47</v>
+        <v>0</v>
       </c>
       <c r="AD7" s="7">
         <f>BCEU_consumoBTU!AF10*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>136208542422416.91</v>
+        <v>0</v>
       </c>
       <c r="AE7" s="7">
         <f>BCEU_consumoBTU!AG10*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>135527499710304.81</v>
+        <v>0</v>
       </c>
       <c r="AF7" s="7">
         <f>BCEU_consumoBTU!AH10*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>134849862211753.3</v>
+        <v>0</v>
       </c>
       <c r="AG7" s="7">
         <f>BCEU_consumoBTU!AI10*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>134175612900694.53</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.2">
@@ -10719,131 +10719,131 @@
       </c>
       <c r="B10" s="7">
         <f>BCEU_consumoBTU!D13*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>163408596240934.38</v>
+        <v>9804515774456.0625</v>
       </c>
       <c r="C10" s="7">
         <f>BCEU_consumoBTU!E13*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>163188443197834.44</v>
+        <v>9791306591870.0664</v>
       </c>
       <c r="D10" s="7">
         <f>BCEU_consumoBTU!F13*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>163133404937059.44</v>
+        <v>9788004296223.5664</v>
       </c>
       <c r="E10" s="7">
         <f>BCEU_consumoBTU!G13*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>162940771024347</v>
+        <v>9776446261460.8203</v>
       </c>
       <c r="F10" s="7">
         <f>BCEU_consumoBTU!H13*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>162665579720472.09</v>
+        <v>9759934783228.3262</v>
       </c>
       <c r="G10" s="7">
         <f>BCEU_consumoBTU!I13*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>162500464938147.09</v>
+        <v>9750027896288.8262</v>
       </c>
       <c r="H10" s="7">
         <f>BCEU_consumoBTU!J13*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>162335350155822.16</v>
+        <v>9740121009349.3281</v>
       </c>
       <c r="I10" s="7">
         <f>BCEU_consumoBTU!K13*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>162280311895047.19</v>
+        <v>9736818713702.8301</v>
       </c>
       <c r="J10" s="7">
         <f>BCEU_consumoBTU!L13*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>162252792764659.66</v>
+        <v>9735167565879.5781</v>
       </c>
       <c r="K10" s="7">
         <f>BCEU_consumoBTU!M13*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>162280311895047.19</v>
+        <v>9736818713702.8301</v>
       </c>
       <c r="L10" s="7">
         <f>BCEU_consumoBTU!N13*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>162335350155822.16</v>
+        <v>9740121009349.3281</v>
       </c>
       <c r="M10" s="7">
         <f>BCEU_consumoBTU!O13*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>162417907546984.66</v>
+        <v>9745074452819.0781</v>
       </c>
       <c r="N10" s="7">
         <f>BCEU_consumoBTU!P13*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>162142716243109.72</v>
+        <v>9728562974586.582</v>
       </c>
       <c r="O10" s="7">
         <f>BCEU_consumoBTU!Q13*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>161332002661894.16</v>
+        <v>9679920159713.6484</v>
       </c>
       <c r="P10" s="7">
         <f>BCEU_consumoBTU!R13*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>160525342648584.66</v>
+        <v>9631520558915.0781</v>
       </c>
       <c r="Q10" s="7">
         <f>BCEU_consumoBTU!S13*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>159722715935341.75</v>
+        <v>9583362956120.5039</v>
       </c>
       <c r="R10" s="7">
         <f>BCEU_consumoBTU!T13*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>158924102355665.03</v>
+        <v>9535446141339.9023</v>
       </c>
       <c r="S10" s="7">
         <f>BCEU_consumoBTU!U13*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>158129481843886.69</v>
+        <v>9487768910633.2012</v>
       </c>
       <c r="T10" s="7">
         <f>BCEU_consumoBTU!V13*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>157338834434667.25</v>
+        <v>9440330066080.0352</v>
       </c>
       <c r="U10" s="7">
         <f>BCEU_consumoBTU!W13*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>156552140262493.91</v>
+        <v>9393128415749.6348</v>
       </c>
       <c r="V10" s="7">
         <f>BCEU_consumoBTU!X13*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>155769379561181.44</v>
+        <v>9346162773670.8867</v>
       </c>
       <c r="W10" s="7">
         <f>BCEU_consumoBTU!Y13*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>154990532663375.53</v>
+        <v>9299431959802.5312</v>
       </c>
       <c r="X10" s="7">
         <f>BCEU_consumoBTU!Z13*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>154215580000058.66</v>
+        <v>9252934800003.5195</v>
       </c>
       <c r="Y10" s="7">
         <f>BCEU_consumoBTU!AA13*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>153444502100058.38</v>
+        <v>9206670126003.502</v>
       </c>
       <c r="Z10" s="7">
         <f>BCEU_consumoBTU!AB13*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>152677279589558.09</v>
+        <v>9160636775373.4844</v>
       </c>
       <c r="AA10" s="7">
         <f>BCEU_consumoBTU!AC13*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>151913893191610.28</v>
+        <v>9114833591496.6172</v>
       </c>
       <c r="AB10" s="7">
         <f>BCEU_consumoBTU!AD13*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>151154323725652.25</v>
+        <v>9069259423539.1348</v>
       </c>
       <c r="AC10" s="7">
         <f>BCEU_consumoBTU!AE13*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>150398552107023.97</v>
+        <v>9023913126421.4375</v>
       </c>
       <c r="AD10" s="7">
         <f>BCEU_consumoBTU!AF13*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>149646559346488.88</v>
+        <v>8978793560789.332</v>
       </c>
       <c r="AE10" s="7">
         <f>BCEU_consumoBTU!AG13*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>148898326549756.41</v>
+        <v>8933899592985.3848</v>
       </c>
       <c r="AF10" s="7">
         <f>BCEU_consumoBTU!AH13*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>148153834917007.62</v>
+        <v>8889230095020.457</v>
       </c>
       <c r="AG10" s="7">
         <f>BCEU_consumoBTU!AI13*'BNE Fuel &amp; component splits'!$B$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>147413065742422.56</v>
+        <v>8844783944545.3535</v>
       </c>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.2">
@@ -14380,131 +14380,131 @@
       </c>
       <c r="B4" s="7">
         <f>BCEU_consumoBTU!D7*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>19904979459089.266</v>
       </c>
       <c r="C4" s="7">
         <f>BCEU_consumoBTU!E7*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>19987608202907.418</v>
       </c>
       <c r="D4" s="7">
         <f>BCEU_consumoBTU!F7*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>20078784747810.203</v>
       </c>
       <c r="E4" s="7">
         <f>BCEU_consumoBTU!G7*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>20147167156487.293</v>
       </c>
       <c r="F4" s="7">
         <f>BCEU_consumoBTU!H7*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>20195604695966.898</v>
       </c>
       <c r="G4" s="7">
         <f>BCEU_consumoBTU!I7*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>20252590036531.137</v>
       </c>
       <c r="H4" s="7">
         <f>BCEU_consumoBTU!J7*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>20301027576010.738</v>
       </c>
       <c r="I4" s="7">
         <f>BCEU_consumoBTU!K7*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>20358012916574.98</v>
       </c>
       <c r="J4" s="7">
         <f>BCEU_consumoBTU!L7*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>20412148990111.012</v>
       </c>
       <c r="K4" s="7">
         <f>BCEU_consumoBTU!M7*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>20469134330675.254</v>
       </c>
       <c r="L4" s="7">
         <f>BCEU_consumoBTU!N7*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>20523270404211.273</v>
       </c>
       <c r="M4" s="7">
         <f>BCEU_consumoBTU!O7*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>20577406477747.309</v>
       </c>
       <c r="N4" s="7">
         <f>BCEU_consumoBTU!P7*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>20571707943690.887</v>
       </c>
       <c r="O4" s="7">
         <f>BCEU_consumoBTU!Q7*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>20880283562846.246</v>
       </c>
       <c r="P4" s="7">
         <f>BCEU_consumoBTU!R7*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>21193487816288.934</v>
       </c>
       <c r="Q4" s="7">
         <f>BCEU_consumoBTU!S7*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>21511390133533.27</v>
       </c>
       <c r="R4" s="7">
         <f>BCEU_consumoBTU!T7*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>21834060985536.27</v>
       </c>
       <c r="S4" s="7">
         <f>BCEU_consumoBTU!U7*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>22161571900319.309</v>
       </c>
       <c r="T4" s="7">
         <f>BCEU_consumoBTU!V7*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>22493995478824.094</v>
       </c>
       <c r="U4" s="7">
         <f>BCEU_consumoBTU!W7*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>22831405411006.461</v>
       </c>
       <c r="V4" s="7">
         <f>BCEU_consumoBTU!X7*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>23173876492171.551</v>
       </c>
       <c r="W4" s="7">
         <f>BCEU_consumoBTU!Y7*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>23521484639554.121</v>
       </c>
       <c r="X4" s="7">
         <f>BCEU_consumoBTU!Z7*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>23874306909147.434</v>
       </c>
       <c r="Y4" s="7">
         <f>BCEU_consumoBTU!AA7*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>24232421512784.645</v>
       </c>
       <c r="Z4" s="7">
         <f>BCEU_consumoBTU!AB7*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>24595907835476.41</v>
       </c>
       <c r="AA4" s="7">
         <f>BCEU_consumoBTU!AC7*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>24964846453008.555</v>
       </c>
       <c r="AB4" s="7">
         <f>BCEU_consumoBTU!AD7*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>25339319149803.68</v>
       </c>
       <c r="AC4" s="7">
         <f>BCEU_consumoBTU!AE7*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>25719408937050.734</v>
       </c>
       <c r="AD4" s="7">
         <f>BCEU_consumoBTU!AF7*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>26105200071106.488</v>
       </c>
       <c r="AE4" s="7">
         <f>BCEU_consumoBTU!AG7*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>26496778072173.086</v>
       </c>
       <c r="AF4" s="7">
         <f>BCEU_consumoBTU!AH7*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>26894229743255.676</v>
       </c>
       <c r="AG4" s="7">
         <f>BCEU_consumoBTU!AI7*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>27297643189404.516</v>
       </c>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.2">
@@ -14779,131 +14779,131 @@
       </c>
       <c r="B7" s="7">
         <f>BCEU_consumoBTU!D10*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>175344398105357.91</v>
       </c>
       <c r="C7" s="7">
         <f>BCEU_consumoBTU!E10*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>172502311314361.97</v>
       </c>
       <c r="D7" s="7">
         <f>BCEU_consumoBTU!F10*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>170731155777944.22</v>
       </c>
       <c r="E7" s="7">
         <f>BCEU_consumoBTU!G10*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>168095017305136.41</v>
       </c>
       <c r="F7" s="7">
         <f>BCEU_consumoBTU!H10*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>165953154795980.03</v>
       </c>
       <c r="G7" s="7">
         <f>BCEU_consumoBTU!I10*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>163111068004984.09</v>
       </c>
       <c r="H7" s="7">
         <f>BCEU_consumoBTU!J10*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>161339912468566.34</v>
       </c>
       <c r="I7" s="7">
         <f>BCEU_consumoBTU!K10*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>158992101641221.88</v>
       </c>
       <c r="J7" s="7">
         <f>BCEU_consumoBTU!L10*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>156809049468427.91</v>
       </c>
       <c r="K7" s="7">
         <f>BCEU_consumoBTU!M10*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>154131721331982.47</v>
       </c>
       <c r="L7" s="7">
         <f>BCEU_consumoBTU!N10*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>152566514113752.81</v>
       </c>
       <c r="M7" s="7">
         <f>BCEU_consumoBTU!O10*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>149600858331844</v>
       </c>
       <c r="N7" s="7">
         <f>BCEU_consumoBTU!P10*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>147582564813600.5</v>
       </c>
       <c r="O7" s="7">
         <f>BCEU_consumoBTU!Q10*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>146844651989532.53</v>
       </c>
       <c r="P7" s="7">
         <f>BCEU_consumoBTU!R10*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>146110428729584.88</v>
       </c>
       <c r="Q7" s="7">
         <f>BCEU_consumoBTU!S10*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>145379876585936.97</v>
       </c>
       <c r="R7" s="7">
         <f>BCEU_consumoBTU!T10*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>144652977203007.25</v>
       </c>
       <c r="S7" s="7">
         <f>BCEU_consumoBTU!U10*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>143929712316992.22</v>
       </c>
       <c r="T7" s="7">
         <f>BCEU_consumoBTU!V10*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>143210063755407.25</v>
       </c>
       <c r="U7" s="7">
         <f>BCEU_consumoBTU!W10*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>142494013436630.22</v>
       </c>
       <c r="V7" s="7">
         <f>BCEU_consumoBTU!X10*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>141781543369447.06</v>
       </c>
       <c r="W7" s="7">
         <f>BCEU_consumoBTU!Y10*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>141072635652599.84</v>
       </c>
       <c r="X7" s="7">
         <f>BCEU_consumoBTU!Z10*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>140367272474336.83</v>
       </c>
       <c r="Y7" s="7">
         <f>BCEU_consumoBTU!AA10*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>139665436111965.16</v>
       </c>
       <c r="Z7" s="7">
         <f>BCEU_consumoBTU!AB10*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>138967108931405.34</v>
       </c>
       <c r="AA7" s="7">
         <f>BCEU_consumoBTU!AC10*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>138272273386748.3</v>
       </c>
       <c r="AB7" s="7">
         <f>BCEU_consumoBTU!AD10*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>137580912019814.53</v>
       </c>
       <c r="AC7" s="7">
         <f>BCEU_consumoBTU!AE10*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>136893007459715.47</v>
       </c>
       <c r="AD7" s="7">
         <f>BCEU_consumoBTU!AF10*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>136208542422416.91</v>
       </c>
       <c r="AE7" s="7">
         <f>BCEU_consumoBTU!AG10*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>135527499710304.81</v>
       </c>
       <c r="AF7" s="7">
         <f>BCEU_consumoBTU!AH10*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>134849862211753.3</v>
       </c>
       <c r="AG7" s="7">
         <f>BCEU_consumoBTU!AI10*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>134175612900694.53</v>
       </c>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.2">
@@ -15178,131 +15178,131 @@
       </c>
       <c r="B10" s="7">
         <f>BCEU_consumoBTU!D13*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>153604080466478.31</v>
       </c>
       <c r="C10" s="7">
         <f>BCEU_consumoBTU!E13*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>153397136605964.38</v>
       </c>
       <c r="D10" s="7">
         <f>BCEU_consumoBTU!F13*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>153345400640835.88</v>
       </c>
       <c r="E10" s="7">
         <f>BCEU_consumoBTU!G13*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>153164324762886.16</v>
       </c>
       <c r="F10" s="7">
         <f>BCEU_consumoBTU!H13*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>152905644937243.75</v>
       </c>
       <c r="G10" s="7">
         <f>BCEU_consumoBTU!I13*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>152750437041858.25</v>
       </c>
       <c r="H10" s="7">
         <f>BCEU_consumoBTU!J13*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>152595229146472.81</v>
       </c>
       <c r="I10" s="7">
         <f>BCEU_consumoBTU!K13*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>152543493181344.34</v>
       </c>
       <c r="J10" s="7">
         <f>BCEU_consumoBTU!L13*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>152517625198780.06</v>
       </c>
       <c r="K10" s="7">
         <f>BCEU_consumoBTU!M13*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>152543493181344.34</v>
       </c>
       <c r="L10" s="7">
         <f>BCEU_consumoBTU!N13*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>152595229146472.81</v>
       </c>
       <c r="M10" s="7">
         <f>BCEU_consumoBTU!O13*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>152672833094165.56</v>
       </c>
       <c r="N10" s="7">
         <f>BCEU_consumoBTU!P13*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>152414153268523.12</v>
       </c>
       <c r="O10" s="7">
         <f>BCEU_consumoBTU!Q13*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>151652082502180.5</v>
       </c>
       <c r="P10" s="7">
         <f>BCEU_consumoBTU!R13*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>150893822089669.56</v>
       </c>
       <c r="Q10" s="7">
         <f>BCEU_consumoBTU!S13*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>150139352979221.25</v>
       </c>
       <c r="R10" s="7">
         <f>BCEU_consumoBTU!T13*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>149388656214325.12</v>
       </c>
       <c r="S10" s="7">
         <f>BCEU_consumoBTU!U13*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>148641712933253.47</v>
       </c>
       <c r="T10" s="7">
         <f>BCEU_consumoBTU!V13*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>147898504368587.22</v>
       </c>
       <c r="U10" s="7">
         <f>BCEU_consumoBTU!W13*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>147159011846744.25</v>
       </c>
       <c r="V10" s="7">
         <f>BCEU_consumoBTU!X13*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>146423216787510.53</v>
       </c>
       <c r="W10" s="7">
         <f>BCEU_consumoBTU!Y13*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>145691100703573</v>
       </c>
       <c r="X10" s="7">
         <f>BCEU_consumoBTU!Z13*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>144962645200055.12</v>
       </c>
       <c r="Y10" s="7">
         <f>BCEU_consumoBTU!AA13*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>144237831974054.88</v>
       </c>
       <c r="Z10" s="7">
         <f>BCEU_consumoBTU!AB13*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>143516642814184.59</v>
       </c>
       <c r="AA10" s="7">
         <f>BCEU_consumoBTU!AC13*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>142799059600113.66</v>
       </c>
       <c r="AB10" s="7">
         <f>BCEU_consumoBTU!AD13*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>142085064302113.09</v>
       </c>
       <c r="AC10" s="7">
         <f>BCEU_consumoBTU!AE13*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>141374638980602.53</v>
       </c>
       <c r="AD10" s="7">
         <f>BCEU_consumoBTU!AF13*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>140667765785699.53</v>
       </c>
       <c r="AE10" s="7">
         <f>BCEU_consumoBTU!AG13*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>139964426956771.02</v>
       </c>
       <c r="AF10" s="7">
         <f>BCEU_consumoBTU!AH13*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>139264604821987.16</v>
       </c>
       <c r="AG10" s="7">
         <f>BCEU_consumoBTU!AI13*'BNE Fuel &amp; component splits'!$B$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>138568281797877.2</v>
       </c>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.2">
@@ -17292,131 +17292,131 @@
       </c>
       <c r="B4" s="7">
         <f>BCEU_consumoBTU!D22*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>7202134519319.7969</v>
+        <v>432128071159.18781</v>
       </c>
       <c r="C4" s="7">
         <f>BCEU_consumoBTU!E22*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>7232031728174.6904</v>
+        <v>433921903690.48138</v>
       </c>
       <c r="D4" s="7">
         <f>BCEU_consumoBTU!F22*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>7265021751738.708</v>
+        <v>435901305104.32245</v>
       </c>
       <c r="E4" s="7">
         <f>BCEU_consumoBTU!G22*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>7289764269411.7227</v>
+        <v>437385856164.70337</v>
       </c>
       <c r="F4" s="7">
         <f>BCEU_consumoBTU!H22*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>7307290219430.1074</v>
+        <v>438437413165.80646</v>
       </c>
       <c r="G4" s="7">
         <f>BCEU_consumoBTU!I22*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>7327908984157.6172</v>
+        <v>439674539049.45703</v>
       </c>
       <c r="H4" s="7">
         <f>BCEU_consumoBTU!J22*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>7345434934176.0029</v>
+        <v>440726096050.56018</v>
       </c>
       <c r="I4" s="7">
         <f>BCEU_consumoBTU!K22*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>7366053698903.5156</v>
+        <v>441963221934.21094</v>
       </c>
       <c r="J4" s="7">
         <f>BCEU_consumoBTU!L22*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>7385641525394.6494</v>
+        <v>443138491523.67896</v>
       </c>
       <c r="K4" s="7">
         <f>BCEU_consumoBTU!M22*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>7406260290122.1631</v>
+        <v>444375617407.32977</v>
       </c>
       <c r="L4" s="7">
         <f>BCEU_consumoBTU!N22*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>7425848116613.2979</v>
+        <v>445550886996.79785</v>
       </c>
       <c r="M4" s="7">
         <f>BCEU_consumoBTU!O22*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>7445435943104.4346</v>
+        <v>446726156586.26605</v>
       </c>
       <c r="N4" s="7">
         <f>BCEU_consumoBTU!P22*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>7443374066631.6836</v>
+        <v>446602443997.901</v>
       </c>
       <c r="O4" s="7">
         <f>BCEU_consumoBTU!Q22*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>7555024677631.1572</v>
+        <v>453301480657.86945</v>
       </c>
       <c r="P4" s="7">
         <f>BCEU_consumoBTU!R22*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>7668350047795.625</v>
+        <v>460101002867.73749</v>
       </c>
       <c r="Q4" s="7">
         <f>BCEU_consumoBTU!S22*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>7783375298512.5586</v>
+        <v>467002517910.75348</v>
       </c>
       <c r="R4" s="7">
         <f>BCEU_consumoBTU!T22*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>7900125927990.2461</v>
+        <v>474007555679.41473</v>
       </c>
       <c r="S4" s="7">
         <f>BCEU_consumoBTU!U22*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>8018627816910.0977</v>
+        <v>481117669014.60583</v>
       </c>
       <c r="T4" s="7">
         <f>BCEU_consumoBTU!V22*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>8138907234163.749</v>
+        <v>488334434049.82495</v>
       </c>
       <c r="U4" s="7">
         <f>BCEU_consumoBTU!W22*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>8260990842676.2061</v>
+        <v>495659450560.57233</v>
       </c>
       <c r="V4" s="7">
         <f>BCEU_consumoBTU!X22*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>8384905705316.3477</v>
+        <v>503094342318.98083</v>
       </c>
       <c r="W4" s="7">
         <f>BCEU_consumoBTU!Y22*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>8510679290896.0918</v>
+        <v>510640757453.7655</v>
       </c>
       <c r="X4" s="7">
         <f>BCEU_consumoBTU!Z22*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>8638339480259.5342</v>
+        <v>518300368815.57202</v>
       </c>
       <c r="Y4" s="7">
         <f>BCEU_consumoBTU!AA22*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>8767914572463.4258</v>
+        <v>526074874347.80554</v>
       </c>
       <c r="Z4" s="7">
         <f>BCEU_consumoBTU!AB22*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>8899433291050.375</v>
+        <v>533965997463.02246</v>
       </c>
       <c r="AA4" s="7">
         <f>BCEU_consumoBTU!AC22*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>9032924790416.1309</v>
+        <v>541975487424.96783</v>
       </c>
       <c r="AB4" s="7">
         <f>BCEU_consumoBTU!AD22*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>9168418662272.3711</v>
+        <v>550105119736.34229</v>
       </c>
       <c r="AC4" s="7">
         <f>BCEU_consumoBTU!AE22*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>9305944942206.457</v>
+        <v>558356696532.38745</v>
       </c>
       <c r="AD4" s="7">
         <f>BCEU_consumoBTU!AF22*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>9445534116339.5527</v>
+        <v>566732046980.37317</v>
       </c>
       <c r="AE4" s="7">
         <f>BCEU_consumoBTU!AG22*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>9587217128084.6445</v>
+        <v>575233027685.07861</v>
       </c>
       <c r="AF4" s="7">
         <f>BCEU_consumoBTU!AH22*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>9731025385005.9141</v>
+        <v>583861523100.35486</v>
       </c>
       <c r="AG4" s="7">
         <f>BCEU_consumoBTU!AI22*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B48</f>
-        <v>9876990765781.002</v>
+        <v>592619445946.86011</v>
       </c>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.2">
@@ -17691,131 +17691,131 @@
       </c>
       <c r="B7" s="7">
         <f>BCEU_consumoBTU!D25*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>59637474545599.359</v>
+        <v>0</v>
       </c>
       <c r="C7" s="7">
         <f>BCEU_consumoBTU!E25*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>58670834718574.141</v>
+        <v>0</v>
       </c>
       <c r="D7" s="7">
         <f>BCEU_consumoBTU!F25*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>58068435985790.312</v>
+        <v>0</v>
       </c>
       <c r="E7" s="7">
         <f>BCEU_consumoBTU!G25*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>57171842523042.281</v>
+        <v>0</v>
       </c>
       <c r="F7" s="7">
         <f>BCEU_consumoBTU!H25*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>56443360334559.5</v>
+        <v>0</v>
       </c>
       <c r="G7" s="7">
         <f>BCEU_consumoBTU!I25*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>55476720507534.289</v>
+        <v>0</v>
       </c>
       <c r="H7" s="7">
         <f>BCEU_consumoBTU!J25*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>54874321774750.453</v>
+        <v>0</v>
       </c>
       <c r="I7" s="7">
         <f>BCEU_consumoBTU!K25*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>54075793221990.492</v>
+        <v>0</v>
       </c>
       <c r="J7" s="7">
         <f>BCEU_consumoBTU!L25*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>53333301760652.281</v>
+        <v>0</v>
       </c>
       <c r="K7" s="7">
         <f>BCEU_consumoBTU!M25*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>52422699025048.812</v>
+        <v>0</v>
       </c>
       <c r="L7" s="7">
         <f>BCEU_consumoBTU!N25*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>51890346656542.164</v>
+        <v>0</v>
       </c>
       <c r="M7" s="7">
         <f>BCEU_consumoBTU!O25*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>50881679010950.633</v>
+        <v>0</v>
       </c>
       <c r="N7" s="7">
         <f>BCEU_consumoBTU!P25*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>50195224641034.172</v>
+        <v>0</v>
       </c>
       <c r="O7" s="7">
         <f>BCEU_consumoBTU!Q25*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>49944248517829.008</v>
+        <v>0</v>
       </c>
       <c r="P7" s="7">
         <f>BCEU_consumoBTU!R25*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>49694527275239.867</v>
+        <v>0</v>
       </c>
       <c r="Q7" s="7">
         <f>BCEU_consumoBTU!S25*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>49446054638863.672</v>
+        <v>0</v>
       </c>
       <c r="R7" s="7">
         <f>BCEU_consumoBTU!T25*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>49198824365669.344</v>
+        <v>0</v>
       </c>
       <c r="S7" s="7">
         <f>BCEU_consumoBTU!U25*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>48952830243841.008</v>
+        <v>0</v>
       </c>
       <c r="T7" s="7">
         <f>BCEU_consumoBTU!V25*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>48708066092621.797</v>
+        <v>0</v>
       </c>
       <c r="U7" s="7">
         <f>BCEU_consumoBTU!W25*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>48464525762158.688</v>
+        <v>0</v>
       </c>
       <c r="V7" s="7">
         <f>BCEU_consumoBTU!X25*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>48222203133347.891</v>
+        <v>0</v>
       </c>
       <c r="W7" s="7">
         <f>BCEU_consumoBTU!Y25*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>47981092117681.156</v>
+        <v>0</v>
       </c>
       <c r="X7" s="7">
         <f>BCEU_consumoBTU!Z25*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>47741186657092.75</v>
+        <v>0</v>
       </c>
       <c r="Y7" s="7">
         <f>BCEU_consumoBTU!AA25*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>47502480723807.281</v>
+        <v>0</v>
       </c>
       <c r="Z7" s="7">
         <f>BCEU_consumoBTU!AB25*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>47264968320188.25</v>
+        <v>0</v>
       </c>
       <c r="AA7" s="7">
         <f>BCEU_consumoBTU!AC25*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>47028643478587.297</v>
+        <v>0</v>
       </c>
       <c r="AB7" s="7">
         <f>BCEU_consumoBTU!AD25*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>46793500261194.367</v>
+        <v>0</v>
       </c>
       <c r="AC7" s="7">
         <f>BCEU_consumoBTU!AE25*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>46559532759888.391</v>
+        <v>0</v>
       </c>
       <c r="AD7" s="7">
         <f>BCEU_consumoBTU!AF25*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>46326735096088.953</v>
+        <v>0</v>
       </c>
       <c r="AE7" s="7">
         <f>BCEU_consumoBTU!AG25*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>46095101420608.516</v>
+        <v>0</v>
       </c>
       <c r="AF7" s="7">
         <f>BCEU_consumoBTU!AH25*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>45864625913505.469</v>
+        <v>0</v>
       </c>
       <c r="AG7" s="7">
         <f>BCEU_consumoBTU!AI25*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B51</f>
-        <v>45635302783937.945</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.2">
@@ -18090,131 +18090,131 @@
       </c>
       <c r="B10" s="7">
         <f>BCEU_consumoBTU!D28*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>55577914687615.359</v>
+        <v>3334674881256.9214</v>
       </c>
       <c r="C10" s="7">
         <f>BCEU_consumoBTU!E28*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>55808627474036.906</v>
+        <v>3348517648442.2144</v>
       </c>
       <c r="D10" s="7">
         <f>BCEU_consumoBTU!F28*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>56063207100433.07</v>
+        <v>3363792426025.9839</v>
       </c>
       <c r="E10" s="7">
         <f>BCEU_consumoBTU!G28*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>56254141820230.219</v>
+        <v>3375248509213.813</v>
       </c>
       <c r="F10" s="7">
         <f>BCEU_consumoBTU!H28*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>56389387246753.188</v>
+        <v>3383363234805.1909</v>
       </c>
       <c r="G10" s="7">
         <f>BCEU_consumoBTU!I28*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>56548499513250.781</v>
+        <v>3392909970795.0469</v>
       </c>
       <c r="H10" s="7">
         <f>BCEU_consumoBTU!J28*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>56683744939773.75</v>
+        <v>3401024696386.4248</v>
       </c>
       <c r="I10" s="7">
         <f>BCEU_consumoBTU!K28*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>56842857206271.375</v>
+        <v>3410571432376.2822</v>
       </c>
       <c r="J10" s="7">
         <f>BCEU_consumoBTU!L28*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>56994013859444.094</v>
+        <v>3419640831566.6455</v>
       </c>
       <c r="K10" s="7">
         <f>BCEU_consumoBTU!M28*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>57153126125941.719</v>
+        <v>3429187567556.5029</v>
       </c>
       <c r="L10" s="7">
         <f>BCEU_consumoBTU!N28*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>57304282779114.43</v>
+        <v>3438256966746.8657</v>
       </c>
       <c r="M10" s="7">
         <f>BCEU_consumoBTU!O28*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>57455439432287.172</v>
+        <v>3447326365937.23</v>
       </c>
       <c r="N10" s="7">
         <f>BCEU_consumoBTU!P28*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>57439528205637.414</v>
+        <v>3446371692338.2446</v>
       </c>
       <c r="O10" s="7">
         <f>BCEU_consumoBTU!Q28*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>58301121128721.961</v>
+        <v>3498067267723.3174</v>
       </c>
       <c r="P10" s="7">
         <f>BCEU_consumoBTU!R28*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>59175637945652.781</v>
+        <v>3550538276739.1665</v>
       </c>
       <c r="Q10" s="7">
         <f>BCEU_consumoBTU!S28*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>60063272514837.57</v>
+        <v>3603796350890.2539</v>
       </c>
       <c r="R10" s="7">
         <f>BCEU_consumoBTU!T28*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>60964221602560.141</v>
+        <v>3657853296153.6084</v>
       </c>
       <c r="S10" s="7">
         <f>BCEU_consumoBTU!U28*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>61878684926598.523</v>
+        <v>3712721095595.9111</v>
       </c>
       <c r="T10" s="7">
         <f>BCEU_consumoBTU!V28*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>62806865200497.5</v>
+        <v>3768411912029.8501</v>
       </c>
       <c r="U10" s="7">
         <f>BCEU_consumoBTU!W28*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>63748968178504.961</v>
+        <v>3824938090710.2974</v>
       </c>
       <c r="V10" s="7">
         <f>BCEU_consumoBTU!X28*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>64705202701182.523</v>
+        <v>3882312162070.9512</v>
       </c>
       <c r="W10" s="7">
         <f>BCEU_consumoBTU!Y28*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>65675780741700.266</v>
+        <v>3940546844502.0156</v>
       </c>
       <c r="X10" s="7">
         <f>BCEU_consumoBTU!Z28*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>66660917452825.766</v>
+        <v>3999655047169.5459</v>
       </c>
       <c r="Y10" s="7">
         <f>BCEU_consumoBTU!AA28*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>67660831214618.148</v>
+        <v>4059649872877.0889</v>
       </c>
       <c r="Z10" s="7">
         <f>BCEU_consumoBTU!AB28*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>68675743682837.406</v>
+        <v>4120544620970.2441</v>
       </c>
       <c r="AA10" s="7">
         <f>BCEU_consumoBTU!AC28*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>69705879838079.969</v>
+        <v>4182352790284.7979</v>
       </c>
       <c r="AB10" s="7">
         <f>BCEU_consumoBTU!AD28*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>70751468035651.156</v>
+        <v>4245088082139.0693</v>
       </c>
       <c r="AC10" s="7">
         <f>BCEU_consumoBTU!AE28*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>71812740056185.906</v>
+        <v>4308764403371.1543</v>
       </c>
       <c r="AD10" s="7">
         <f>BCEU_consumoBTU!AF28*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>72889931157028.703</v>
+        <v>4373395869421.7222</v>
       </c>
       <c r="AE10" s="7">
         <f>BCEU_consumoBTU!AG28*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>73983280124384.125</v>
+        <v>4438996807463.0469</v>
       </c>
       <c r="AF10" s="7">
         <f>BCEU_consumoBTU!AH28*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>75093029326249.875</v>
+        <v>4505581759574.9922</v>
       </c>
       <c r="AG10" s="7">
         <f>BCEU_consumoBTU!AI28*'BNE Fuel &amp; component splits'!$C$37*'BNE Fuel &amp; component splits'!$B54</f>
-        <v>76219424766143.609</v>
+        <v>4573165485968.6162</v>
       </c>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.2">
@@ -21663,131 +21663,131 @@
       </c>
       <c r="B4" s="7">
         <f>BCEU_consumoBTU!D22*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>6770006448160.6094</v>
       </c>
       <c r="C4" s="7">
         <f>BCEU_consumoBTU!E22*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>6798109824484.209</v>
       </c>
       <c r="D4" s="7">
         <f>BCEU_consumoBTU!F22*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>6829120446634.3857</v>
       </c>
       <c r="E4" s="7">
         <f>BCEU_consumoBTU!G22*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>6852378413247.0195</v>
       </c>
       <c r="F4" s="7">
         <f>BCEU_consumoBTU!H22*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>6868852806264.3018</v>
       </c>
       <c r="G4" s="7">
         <f>BCEU_consumoBTU!I22*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>6888234445108.1602</v>
       </c>
       <c r="H4" s="7">
         <f>BCEU_consumoBTU!J22*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>6904708838125.4434</v>
       </c>
       <c r="I4" s="7">
         <f>BCEU_consumoBTU!K22*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>6924090476969.3047</v>
       </c>
       <c r="J4" s="7">
         <f>BCEU_consumoBTU!L22*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>6942503033870.9707</v>
       </c>
       <c r="K4" s="7">
         <f>BCEU_consumoBTU!M22*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>6961884672714.834</v>
       </c>
       <c r="L4" s="7">
         <f>BCEU_consumoBTU!N22*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>6980297229616.5</v>
       </c>
       <c r="M4" s="7">
         <f>BCEU_consumoBTU!O22*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>6998709786518.1689</v>
       </c>
       <c r="N4" s="7">
         <f>BCEU_consumoBTU!P22*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>6996771622633.7832</v>
       </c>
       <c r="O4" s="7">
         <f>BCEU_consumoBTU!Q22*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>7101723196973.2881</v>
       </c>
       <c r="P4" s="7">
         <f>BCEU_consumoBTU!R22*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>7208249044927.8877</v>
       </c>
       <c r="Q4" s="7">
         <f>BCEU_consumoBTU!S22*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>7316372780601.8057</v>
       </c>
       <c r="R4" s="7">
         <f>BCEU_consumoBTU!T22*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>7426118372310.832</v>
       </c>
       <c r="S4" s="7">
         <f>BCEU_consumoBTU!U22*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>7537510147895.4922</v>
       </c>
       <c r="T4" s="7">
         <f>BCEU_consumoBTU!V22*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>7650572800113.9248</v>
       </c>
       <c r="U4" s="7">
         <f>BCEU_consumoBTU!W22*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>7765331392115.6338</v>
       </c>
       <c r="V4" s="7">
         <f>BCEU_consumoBTU!X22*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>7881811362997.3672</v>
       </c>
       <c r="W4" s="7">
         <f>BCEU_consumoBTU!Y22*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>8000038533442.3271</v>
       </c>
       <c r="X4" s="7">
         <f>BCEU_consumoBTU!Z22*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>8120039111443.9629</v>
       </c>
       <c r="Y4" s="7">
         <f>BCEU_consumoBTU!AA22*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>8241839698115.6211</v>
       </c>
       <c r="Z4" s="7">
         <f>BCEU_consumoBTU!AB22*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>8365467293587.3525</v>
       </c>
       <c r="AA4" s="7">
         <f>BCEU_consumoBTU!AC22*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>8490949302991.1631</v>
       </c>
       <c r="AB4" s="7">
         <f>BCEU_consumoBTU!AD22*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>8618313542536.0293</v>
       </c>
       <c r="AC4" s="7">
         <f>BCEU_consumoBTU!AE22*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>8747588245674.0703</v>
       </c>
       <c r="AD4" s="7">
         <f>BCEU_consumoBTU!AF22*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>8878802069359.1797</v>
       </c>
       <c r="AE4" s="7">
         <f>BCEU_consumoBTU!AG22*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>9011984100399.5664</v>
       </c>
       <c r="AF4" s="7">
         <f>BCEU_consumoBTU!AH22*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>9147163861905.5605</v>
       </c>
       <c r="AG4" s="7">
         <f>BCEU_consumoBTU!AI22*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E48</f>
-        <v>0</v>
+        <v>9284371319834.1426</v>
       </c>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.2">
@@ -22062,131 +22062,131 @@
       </c>
       <c r="B7" s="7">
         <f>BCEU_consumoBTU!D25*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>59637474545599.359</v>
       </c>
       <c r="C7" s="7">
         <f>BCEU_consumoBTU!E25*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>58670834718574.141</v>
       </c>
       <c r="D7" s="7">
         <f>BCEU_consumoBTU!F25*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>58068435985790.312</v>
       </c>
       <c r="E7" s="7">
         <f>BCEU_consumoBTU!G25*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>57171842523042.281</v>
       </c>
       <c r="F7" s="7">
         <f>BCEU_consumoBTU!H25*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>56443360334559.5</v>
       </c>
       <c r="G7" s="7">
         <f>BCEU_consumoBTU!I25*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>55476720507534.289</v>
       </c>
       <c r="H7" s="7">
         <f>BCEU_consumoBTU!J25*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>54874321774750.453</v>
       </c>
       <c r="I7" s="7">
         <f>BCEU_consumoBTU!K25*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>54075793221990.492</v>
       </c>
       <c r="J7" s="7">
         <f>BCEU_consumoBTU!L25*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>53333301760652.281</v>
       </c>
       <c r="K7" s="7">
         <f>BCEU_consumoBTU!M25*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>52422699025048.812</v>
       </c>
       <c r="L7" s="7">
         <f>BCEU_consumoBTU!N25*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>51890346656542.164</v>
       </c>
       <c r="M7" s="7">
         <f>BCEU_consumoBTU!O25*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>50881679010950.633</v>
       </c>
       <c r="N7" s="7">
         <f>BCEU_consumoBTU!P25*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>50195224641034.172</v>
       </c>
       <c r="O7" s="7">
         <f>BCEU_consumoBTU!Q25*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>49944248517829.008</v>
       </c>
       <c r="P7" s="7">
         <f>BCEU_consumoBTU!R25*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>49694527275239.867</v>
       </c>
       <c r="Q7" s="7">
         <f>BCEU_consumoBTU!S25*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>49446054638863.672</v>
       </c>
       <c r="R7" s="7">
         <f>BCEU_consumoBTU!T25*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>49198824365669.344</v>
       </c>
       <c r="S7" s="7">
         <f>BCEU_consumoBTU!U25*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>48952830243841.008</v>
       </c>
       <c r="T7" s="7">
         <f>BCEU_consumoBTU!V25*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>48708066092621.797</v>
       </c>
       <c r="U7" s="7">
         <f>BCEU_consumoBTU!W25*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>48464525762158.688</v>
       </c>
       <c r="V7" s="7">
         <f>BCEU_consumoBTU!X25*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>48222203133347.891</v>
       </c>
       <c r="W7" s="7">
         <f>BCEU_consumoBTU!Y25*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>47981092117681.156</v>
       </c>
       <c r="X7" s="7">
         <f>BCEU_consumoBTU!Z25*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>47741186657092.75</v>
       </c>
       <c r="Y7" s="7">
         <f>BCEU_consumoBTU!AA25*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>47502480723807.281</v>
       </c>
       <c r="Z7" s="7">
         <f>BCEU_consumoBTU!AB25*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>47264968320188.25</v>
       </c>
       <c r="AA7" s="7">
         <f>BCEU_consumoBTU!AC25*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>47028643478587.297</v>
       </c>
       <c r="AB7" s="7">
         <f>BCEU_consumoBTU!AD25*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>46793500261194.367</v>
       </c>
       <c r="AC7" s="7">
         <f>BCEU_consumoBTU!AE25*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>46559532759888.391</v>
       </c>
       <c r="AD7" s="7">
         <f>BCEU_consumoBTU!AF25*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>46326735096088.953</v>
       </c>
       <c r="AE7" s="7">
         <f>BCEU_consumoBTU!AG25*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>46095101420608.516</v>
       </c>
       <c r="AF7" s="7">
         <f>BCEU_consumoBTU!AH25*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>45864625913505.469</v>
       </c>
       <c r="AG7" s="7">
         <f>BCEU_consumoBTU!AI25*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E51</f>
-        <v>0</v>
+        <v>45635302783937.945</v>
       </c>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.2">
@@ -22461,131 +22461,131 @@
       </c>
       <c r="B10" s="7">
         <f>BCEU_consumoBTU!D28*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>52243239806358.438</v>
       </c>
       <c r="C10" s="7">
         <f>BCEU_consumoBTU!E28*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>52460109825594.688</v>
       </c>
       <c r="D10" s="7">
         <f>BCEU_consumoBTU!F28*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>52699414674407.086</v>
       </c>
       <c r="E10" s="7">
         <f>BCEU_consumoBTU!G28*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>52878893311016.406</v>
       </c>
       <c r="F10" s="7">
         <f>BCEU_consumoBTU!H28*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>53006024011947.992</v>
       </c>
       <c r="G10" s="7">
         <f>BCEU_consumoBTU!I28*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>53155589542455.734</v>
       </c>
       <c r="H10" s="7">
         <f>BCEU_consumoBTU!J28*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>53282720243387.32</v>
       </c>
       <c r="I10" s="7">
         <f>BCEU_consumoBTU!K28*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>53432285773895.086</v>
       </c>
       <c r="J10" s="7">
         <f>BCEU_consumoBTU!L28*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>53574373027877.445</v>
       </c>
       <c r="K10" s="7">
         <f>BCEU_consumoBTU!M28*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>53723938558385.211</v>
       </c>
       <c r="L10" s="7">
         <f>BCEU_consumoBTU!N28*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>53866025812367.562</v>
       </c>
       <c r="M10" s="7">
         <f>BCEU_consumoBTU!O28*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>54008113066349.938</v>
       </c>
       <c r="N10" s="7">
         <f>BCEU_consumoBTU!P28*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>53993156513299.164</v>
       </c>
       <c r="O10" s="7">
         <f>BCEU_consumoBTU!Q28*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>54803053860998.641</v>
       </c>
       <c r="P10" s="7">
         <f>BCEU_consumoBTU!R28*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>55625099668913.609</v>
       </c>
       <c r="Q10" s="7">
         <f>BCEU_consumoBTU!S28*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>56459476163947.312</v>
       </c>
       <c r="R10" s="7">
         <f>BCEU_consumoBTU!T28*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>57306368306406.531</v>
       </c>
       <c r="S10" s="7">
         <f>BCEU_consumoBTU!U28*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>58165963831002.609</v>
       </c>
       <c r="T10" s="7">
         <f>BCEU_consumoBTU!V28*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>59038453288467.648</v>
       </c>
       <c r="U10" s="7">
         <f>BCEU_consumoBTU!W28*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>59924030087794.656</v>
       </c>
       <c r="V10" s="7">
         <f>BCEU_consumoBTU!X28*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>60822890539111.57</v>
       </c>
       <c r="W10" s="7">
         <f>BCEU_consumoBTU!Y28*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>61735233897198.25</v>
       </c>
       <c r="X10" s="7">
         <f>BCEU_consumoBTU!Z28*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>62661262405656.219</v>
       </c>
       <c r="Y10" s="7">
         <f>BCEU_consumoBTU!AA28*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>63601181341741.055</v>
       </c>
       <c r="Z10" s="7">
         <f>BCEU_consumoBTU!AB28*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>64555199061867.156</v>
       </c>
       <c r="AA10" s="7">
         <f>BCEU_consumoBTU!AC28*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>65523527047795.164</v>
       </c>
       <c r="AB10" s="7">
         <f>BCEU_consumoBTU!AD28*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>66506379953512.086</v>
       </c>
       <c r="AC10" s="7">
         <f>BCEU_consumoBTU!AE28*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>67503975652814.75</v>
       </c>
       <c r="AD10" s="7">
         <f>BCEU_consumoBTU!AF28*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>68516535287606.977</v>
       </c>
       <c r="AE10" s="7">
         <f>BCEU_consumoBTU!AG28*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>69544283316921.07</v>
       </c>
       <c r="AF10" s="7">
         <f>BCEU_consumoBTU!AH28*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>70587447566674.875</v>
       </c>
       <c r="AG10" s="7">
         <f>BCEU_consumoBTU!AI28*'BNE Fuel &amp; component splits'!$C$40*'BNE Fuel &amp; component splits'!$E54</f>
-        <v>0</v>
+        <v>71646259280174.984</v>
       </c>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.2">
@@ -24482,24 +24482,24 @@
       <c r="Q29" s="25"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A30" s="110" t="s">
+      <c r="A30" s="113" t="s">
         <v>76</v>
       </c>
-      <c r="B30" s="111"/>
-      <c r="C30" s="111"/>
-      <c r="D30" s="111"/>
-      <c r="E30" s="111"/>
-      <c r="F30" s="111"/>
-      <c r="G30" s="111"/>
-      <c r="H30" s="111"/>
-      <c r="I30" s="111"/>
-      <c r="J30" s="111"/>
-      <c r="K30" s="111"/>
-      <c r="L30" s="111"/>
-      <c r="M30" s="111"/>
-      <c r="N30" s="111"/>
-      <c r="O30" s="111"/>
-      <c r="P30" s="111"/>
+      <c r="B30" s="114"/>
+      <c r="C30" s="114"/>
+      <c r="D30" s="114"/>
+      <c r="E30" s="114"/>
+      <c r="F30" s="114"/>
+      <c r="G30" s="114"/>
+      <c r="H30" s="114"/>
+      <c r="I30" s="114"/>
+      <c r="J30" s="114"/>
+      <c r="K30" s="114"/>
+      <c r="L30" s="114"/>
+      <c r="M30" s="114"/>
+      <c r="N30" s="114"/>
+      <c r="O30" s="114"/>
+      <c r="P30" s="114"/>
       <c r="Q30" s="28" t="s">
         <v>77</v>
       </c>
@@ -24921,14 +24921,14 @@
       <c r="G46" s="25"/>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A47" s="110" t="s">
+      <c r="A47" s="113" t="s">
         <v>101</v>
       </c>
-      <c r="B47" s="111"/>
-      <c r="C47" s="111"/>
-      <c r="D47" s="111"/>
-      <c r="E47" s="111"/>
-      <c r="F47" s="111"/>
+      <c r="B47" s="114"/>
+      <c r="C47" s="114"/>
+      <c r="D47" s="114"/>
+      <c r="E47" s="114"/>
+      <c r="F47" s="114"/>
       <c r="G47" s="28" t="s">
         <v>102</v>
       </c>
@@ -26080,17 +26080,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="E49:G49"/>
     <mergeCell ref="A47:F47"/>
     <mergeCell ref="A30:P30"/>
     <mergeCell ref="A32:A33"/>
     <mergeCell ref="B32:B33"/>
     <mergeCell ref="C32:C33"/>
     <mergeCell ref="D32:Q32"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="E49:G49"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="Q27" location="Índice!A1" display="Índice" xr:uid="{BEE6A9BA-4DAC-1B47-B244-0354F97CEB5B}"/>
@@ -26496,131 +26496,131 @@
       </c>
       <c r="B4" s="7">
         <f>BCEU_consumoBTU!D37*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B61</f>
-        <v>10389971272874.584</v>
+        <v>4155988509149.834</v>
       </c>
       <c r="C4" s="7">
         <f>BCEU_consumoBTU!E37*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B61</f>
-        <v>10433101700431.609</v>
+        <v>4173240680172.644</v>
       </c>
       <c r="D4" s="7">
         <f>BCEU_consumoBTU!F37*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B61</f>
-        <v>10480693896356.6</v>
+        <v>4192277558542.6401</v>
       </c>
       <c r="E4" s="7">
         <f>BCEU_consumoBTU!G37*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B61</f>
-        <v>10516388043300.344</v>
+        <v>4206555217320.1377</v>
       </c>
       <c r="F4" s="7">
         <f>BCEU_consumoBTU!H37*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B61</f>
-        <v>10541671397385.496</v>
+        <v>4216668558954.1987</v>
       </c>
       <c r="G4" s="7">
         <f>BCEU_consumoBTU!I37*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B61</f>
-        <v>10571416519838.611</v>
+        <v>4228566607935.4448</v>
       </c>
       <c r="H4" s="7">
         <f>BCEU_consumoBTU!J37*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B61</f>
-        <v>10596699873923.764</v>
+        <v>4238679949569.5059</v>
       </c>
       <c r="I4" s="7">
         <f>BCEU_consumoBTU!K37*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B61</f>
-        <v>10626444996376.885</v>
+        <v>4250577998550.7539</v>
       </c>
       <c r="J4" s="7">
         <f>BCEU_consumoBTU!L37*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B61</f>
-        <v>10654702862707.346</v>
+        <v>4261881145082.9385</v>
       </c>
       <c r="K4" s="7">
         <f>BCEU_consumoBTU!M37*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B61</f>
-        <v>10684447985160.467</v>
+        <v>4273779194064.187</v>
       </c>
       <c r="L4" s="7">
         <f>BCEU_consumoBTU!N37*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B61</f>
-        <v>10712705851490.93</v>
+        <v>4285082340596.3721</v>
       </c>
       <c r="M4" s="7">
         <f>BCEU_consumoBTU!O37*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B61</f>
-        <v>10740963717821.395</v>
+        <v>4296385487128.5581</v>
       </c>
       <c r="N4" s="7">
         <f>BCEU_consumoBTU!P37*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B61</f>
-        <v>10737989205576.082</v>
+        <v>4295195682230.4331</v>
       </c>
       <c r="O4" s="7">
         <f>BCEU_consumoBTU!Q37*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B61</f>
-        <v>10899059043659.721</v>
+        <v>4359623617463.8887</v>
       </c>
       <c r="P4" s="7">
         <f>BCEU_consumoBTU!R37*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B61</f>
-        <v>11062544929314.615</v>
+        <v>4425017971725.8467</v>
       </c>
       <c r="Q4" s="7">
         <f>BCEU_consumoBTU!S37*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B61</f>
-        <v>11228483103254.334</v>
+        <v>4491393241301.7334</v>
       </c>
       <c r="R4" s="7">
         <f>BCEU_consumoBTU!T37*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B61</f>
-        <v>11396910349803.15</v>
+        <v>4558764139921.2607</v>
       </c>
       <c r="S4" s="7">
         <f>BCEU_consumoBTU!U37*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B61</f>
-        <v>11567864005050.193</v>
+        <v>4627145602020.0771</v>
       </c>
       <c r="T4" s="7">
         <f>BCEU_consumoBTU!V37*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B61</f>
-        <v>11741381965125.947</v>
+        <v>4696552786050.3789</v>
       </c>
       <c r="U4" s="7">
         <f>BCEU_consumoBTU!W37*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B61</f>
-        <v>11917502694602.836</v>
+        <v>4767001077841.1348</v>
       </c>
       <c r="V4" s="7">
         <f>BCEU_consumoBTU!X37*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B61</f>
-        <v>12096265235021.877</v>
+        <v>4838506094008.751</v>
       </c>
       <c r="W4" s="7">
         <f>BCEU_consumoBTU!Y37*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B61</f>
-        <v>12277709213547.205</v>
+        <v>4911083685418.8818</v>
       </c>
       <c r="X4" s="7">
         <f>BCEU_consumoBTU!Z37*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B61</f>
-        <v>12461874851750.412</v>
+        <v>4984749940700.165</v>
       </c>
       <c r="Y4" s="7">
         <f>BCEU_consumoBTU!AA37*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B61</f>
-        <v>12648802974526.666</v>
+        <v>5059521189810.667</v>
       </c>
       <c r="Z4" s="7">
         <f>BCEU_consumoBTU!AB37*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B61</f>
-        <v>12838535019144.566</v>
+        <v>5135414007657.8271</v>
       </c>
       <c r="AA4" s="7">
         <f>BCEU_consumoBTU!AC37*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B61</f>
-        <v>13031113044431.732</v>
+        <v>5212445217772.6934</v>
       </c>
       <c r="AB4" s="7">
         <f>BCEU_consumoBTU!AD37*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B61</f>
-        <v>13226579740098.205</v>
+        <v>5290631896039.2822</v>
       </c>
       <c r="AC4" s="7">
         <f>BCEU_consumoBTU!AE37*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B61</f>
-        <v>13424978436199.678</v>
+        <v>5369991374479.8711</v>
       </c>
       <c r="AD4" s="7">
         <f>BCEU_consumoBTU!AF37*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B61</f>
-        <v>13626353112742.674</v>
+        <v>5450541245097.0703</v>
       </c>
       <c r="AE4" s="7">
         <f>BCEU_consumoBTU!AG37*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B61</f>
-        <v>13830748409433.811</v>
+        <v>5532299363773.5244</v>
       </c>
       <c r="AF4" s="7">
         <f>BCEU_consumoBTU!AH37*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B61</f>
-        <v>14038209635575.316</v>
+        <v>5615283854230.127</v>
       </c>
       <c r="AG4" s="7">
         <f>BCEU_consumoBTU!AI37*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B61</f>
-        <v>14248782780108.947</v>
+        <v>5699513112043.5791</v>
       </c>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.2">
@@ -27294,131 +27294,131 @@
       </c>
       <c r="B10" s="7">
         <f>BCEU_consumoBTU!D43*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B67</f>
-        <v>58659453759070.898</v>
+        <v>23463781503628.355</v>
       </c>
       <c r="C10" s="7">
         <f>BCEU_consumoBTU!E43*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B67</f>
-        <v>58902958505565.758</v>
+        <v>23561183402226.301</v>
       </c>
       <c r="D10" s="7">
         <f>BCEU_consumoBTU!F43*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B67</f>
-        <v>59171653398249.734</v>
+        <v>23668661359299.891</v>
       </c>
       <c r="E10" s="7">
         <f>BCEU_consumoBTU!G43*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B67</f>
-        <v>59373174567762.727</v>
+        <v>23749269827105.09</v>
       </c>
       <c r="F10" s="7">
         <f>BCEU_consumoBTU!H43*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B67</f>
-        <v>59515918729501.086</v>
+        <v>23806367491800.434</v>
       </c>
       <c r="G10" s="7">
         <f>BCEU_consumoBTU!I43*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B67</f>
-        <v>59683853037428.555</v>
+        <v>23873541214971.418</v>
       </c>
       <c r="H10" s="7">
         <f>BCEU_consumoBTU!J43*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B67</f>
-        <v>59826597199166.922</v>
+        <v>23930638879666.766</v>
       </c>
       <c r="I10" s="7">
         <f>BCEU_consumoBTU!K43*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B67</f>
-        <v>59994531507094.422</v>
+        <v>23997812602837.766</v>
       </c>
       <c r="J10" s="7">
         <f>BCEU_consumoBTU!L43*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B67</f>
-        <v>60154069099625.523</v>
+        <v>24061627639850.207</v>
       </c>
       <c r="K10" s="7">
         <f>BCEU_consumoBTU!M43*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B67</f>
-        <v>60322003407553.023</v>
+        <v>24128801363021.207</v>
       </c>
       <c r="L10" s="7">
         <f>BCEU_consumoBTU!N43*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B67</f>
-        <v>60481541000084.117</v>
+        <v>24192616400033.645</v>
       </c>
       <c r="M10" s="7">
         <f>BCEU_consumoBTU!O43*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B67</f>
-        <v>60641078592615.242</v>
+        <v>24256431437046.094</v>
       </c>
       <c r="N10" s="7">
         <f>BCEU_consumoBTU!P43*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B67</f>
-        <v>60624285161822.492</v>
+        <v>24249714064728.996</v>
       </c>
       <c r="O10" s="7">
         <f>BCEU_consumoBTU!Q43*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B67</f>
-        <v>61533649439249.812</v>
+        <v>24613459775699.922</v>
       </c>
       <c r="P10" s="7">
         <f>BCEU_consumoBTU!R43*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B67</f>
-        <v>62456654180838.555</v>
+        <v>24982661672335.418</v>
       </c>
       <c r="Q10" s="7">
         <f>BCEU_consumoBTU!S43*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B67</f>
-        <v>63393503993551.133</v>
+        <v>25357401597420.449</v>
       </c>
       <c r="R10" s="7">
         <f>BCEU_consumoBTU!T43*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B67</f>
-        <v>64344406553454.398</v>
+        <v>25737762621381.758</v>
       </c>
       <c r="S10" s="7">
         <f>BCEU_consumoBTU!U43*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B67</f>
-        <v>65309572651756.203</v>
+        <v>26123829060702.48</v>
       </c>
       <c r="T10" s="7">
         <f>BCEU_consumoBTU!V43*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B67</f>
-        <v>66289216241532.539</v>
+        <v>26515686496613.012</v>
       </c>
       <c r="U10" s="7">
         <f>BCEU_consumoBTU!W43*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B67</f>
-        <v>67283554485155.539</v>
+        <v>26913421794062.215</v>
       </c>
       <c r="V10" s="7">
         <f>BCEU_consumoBTU!X43*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B67</f>
-        <v>68292807802432.859</v>
+        <v>27317123120973.141</v>
       </c>
       <c r="W10" s="7">
         <f>BCEU_consumoBTU!Y43*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B67</f>
-        <v>69317199919469.352</v>
+        <v>27726879967787.738</v>
       </c>
       <c r="X10" s="7">
         <f>BCEU_consumoBTU!Z43*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B67</f>
-        <v>70356957918261.383</v>
+        <v>28142783167304.551</v>
       </c>
       <c r="Y10" s="7">
         <f>BCEU_consumoBTU!AA43*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B67</f>
-        <v>71412312287035.297</v>
+        <v>28564924914814.117</v>
       </c>
       <c r="Z10" s="7">
         <f>BCEU_consumoBTU!AB43*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B67</f>
-        <v>72483496971340.812</v>
+        <v>28993398788536.324</v>
       </c>
       <c r="AA10" s="7">
         <f>BCEU_consumoBTU!AC43*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B67</f>
-        <v>73570749425910.922</v>
+        <v>29428299770364.367</v>
       </c>
       <c r="AB10" s="7">
         <f>BCEU_consumoBTU!AD43*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B67</f>
-        <v>74674310667299.578</v>
+        <v>29869724266919.828</v>
       </c>
       <c r="AC10" s="7">
         <f>BCEU_consumoBTU!AE43*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B67</f>
-        <v>75794425327309.062</v>
+        <v>30317770130923.621</v>
       </c>
       <c r="AD10" s="7">
         <f>BCEU_consumoBTU!AF43*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B67</f>
-        <v>76931341707218.688</v>
+        <v>30772536682887.473</v>
       </c>
       <c r="AE10" s="7">
         <f>BCEU_consumoBTU!AG43*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B67</f>
-        <v>78085311832826.969</v>
+        <v>31234124733130.785</v>
       </c>
       <c r="AF10" s="7">
         <f>BCEU_consumoBTU!AH43*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B67</f>
-        <v>79256591510319.359</v>
+        <v>31702636604127.742</v>
       </c>
       <c r="AG10" s="7">
         <f>BCEU_consumoBTU!AI43*'BNE Fuel &amp; component splits'!$D$37*'BNE Fuel &amp; component splits'!$B67</f>
-        <v>80445440382974.141</v>
+        <v>32178176153189.652</v>
       </c>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.2">
@@ -30864,131 +30864,131 @@
       </c>
       <c r="B4" s="7">
         <f>BCEU_consumoBTU!D37*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E61</f>
-        <v>0</v>
+        <v>6233982763724.75</v>
       </c>
       <c r="C4" s="7">
         <f>BCEU_consumoBTU!E37*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E61</f>
-        <v>0</v>
+        <v>6259861020258.9658</v>
       </c>
       <c r="D4" s="7">
         <f>BCEU_consumoBTU!F37*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E61</f>
-        <v>0</v>
+        <v>6288416337813.96</v>
       </c>
       <c r="E4" s="7">
         <f>BCEU_consumoBTU!G37*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E61</f>
-        <v>0</v>
+        <v>6309832825980.2061</v>
       </c>
       <c r="F4" s="7">
         <f>BCEU_consumoBTU!H37*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E61</f>
-        <v>0</v>
+        <v>6325002838431.2979</v>
       </c>
       <c r="G4" s="7">
         <f>BCEU_consumoBTU!I37*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E61</f>
-        <v>0</v>
+        <v>6342849911903.167</v>
       </c>
       <c r="H4" s="7">
         <f>BCEU_consumoBTU!J37*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E61</f>
-        <v>0</v>
+        <v>6358019924354.2578</v>
       </c>
       <c r="I4" s="7">
         <f>BCEU_consumoBTU!K37*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E61</f>
-        <v>0</v>
+        <v>6375866997826.1309</v>
       </c>
       <c r="J4" s="7">
         <f>BCEU_consumoBTU!L37*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E61</f>
-        <v>0</v>
+        <v>6392821717624.4072</v>
       </c>
       <c r="K4" s="7">
         <f>BCEU_consumoBTU!M37*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E61</f>
-        <v>0</v>
+        <v>6410668791096.2803</v>
       </c>
       <c r="L4" s="7">
         <f>BCEU_consumoBTU!N37*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E61</f>
-        <v>0</v>
+        <v>6427623510894.5576</v>
       </c>
       <c r="M4" s="7">
         <f>BCEU_consumoBTU!O37*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E61</f>
-        <v>0</v>
+        <v>6444578230692.8369</v>
       </c>
       <c r="N4" s="7">
         <f>BCEU_consumoBTU!P37*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E61</f>
-        <v>0</v>
+        <v>6442793523345.6494</v>
       </c>
       <c r="O4" s="7">
         <f>BCEU_consumoBTU!Q37*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E61</f>
-        <v>0</v>
+        <v>6539435426195.832</v>
       </c>
       <c r="P4" s="7">
         <f>BCEU_consumoBTU!R37*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E61</f>
-        <v>0</v>
+        <v>6637526957588.7686</v>
       </c>
       <c r="Q4" s="7">
         <f>BCEU_consumoBTU!S37*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E61</f>
-        <v>0</v>
+        <v>6737089861952.6006</v>
       </c>
       <c r="R4" s="7">
         <f>BCEU_consumoBTU!T37*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E61</f>
-        <v>0</v>
+        <v>6838146209881.8896</v>
       </c>
       <c r="S4" s="7">
         <f>BCEU_consumoBTU!U37*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E61</f>
-        <v>0</v>
+        <v>6940718403030.1162</v>
       </c>
       <c r="T4" s="7">
         <f>BCEU_consumoBTU!V37*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E61</f>
-        <v>0</v>
+        <v>7044829179075.5684</v>
       </c>
       <c r="U4" s="7">
         <f>BCEU_consumoBTU!W37*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E61</f>
-        <v>0</v>
+        <v>7150501616761.7012</v>
       </c>
       <c r="V4" s="7">
         <f>BCEU_consumoBTU!X37*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E61</f>
-        <v>0</v>
+        <v>7257759141013.126</v>
       </c>
       <c r="W4" s="7">
         <f>BCEU_consumoBTU!Y37*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E61</f>
-        <v>0</v>
+        <v>7366625528128.3232</v>
       </c>
       <c r="X4" s="7">
         <f>BCEU_consumoBTU!Z37*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E61</f>
-        <v>0</v>
+        <v>7477124911050.2471</v>
       </c>
       <c r="Y4" s="7">
         <f>BCEU_consumoBTU!AA37*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E61</f>
-        <v>0</v>
+        <v>7589281784715.999</v>
       </c>
       <c r="Z4" s="7">
         <f>BCEU_consumoBTU!AB37*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E61</f>
-        <v>0</v>
+        <v>7703121011486.7393</v>
       </c>
       <c r="AA4" s="7">
         <f>BCEU_consumoBTU!AC37*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E61</f>
-        <v>0</v>
+        <v>7818667826659.0391</v>
       </c>
       <c r="AB4" s="7">
         <f>BCEU_consumoBTU!AD37*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E61</f>
-        <v>0</v>
+        <v>7935947844058.9229</v>
       </c>
       <c r="AC4" s="7">
         <f>BCEU_consumoBTU!AE37*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E61</f>
-        <v>0</v>
+        <v>8054987061719.8066</v>
       </c>
       <c r="AD4" s="7">
         <f>BCEU_consumoBTU!AF37*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E61</f>
-        <v>0</v>
+        <v>8175811867645.6035</v>
       </c>
       <c r="AE4" s="7">
         <f>BCEU_consumoBTU!AG37*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E61</f>
-        <v>0</v>
+        <v>8298449045660.2861</v>
       </c>
       <c r="AF4" s="7">
         <f>BCEU_consumoBTU!AH37*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E61</f>
-        <v>0</v>
+        <v>8422925781345.1895</v>
       </c>
       <c r="AG4" s="7">
         <f>BCEU_consumoBTU!AI37*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E61</f>
-        <v>0</v>
+        <v>8549269668065.3682</v>
       </c>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.2">
@@ -31662,131 +31662,131 @@
       </c>
       <c r="B10" s="7">
         <f>BCEU_consumoBTU!D43*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E67</f>
-        <v>0</v>
+        <v>35195672255442.539</v>
       </c>
       <c r="C10" s="7">
         <f>BCEU_consumoBTU!E43*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E67</f>
-        <v>0</v>
+        <v>35341775103339.453</v>
       </c>
       <c r="D10" s="7">
         <f>BCEU_consumoBTU!F43*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E67</f>
-        <v>0</v>
+        <v>35502992038949.836</v>
       </c>
       <c r="E10" s="7">
         <f>BCEU_consumoBTU!G43*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E67</f>
-        <v>0</v>
+        <v>35623904740657.633</v>
       </c>
       <c r="F10" s="7">
         <f>BCEU_consumoBTU!H43*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E67</f>
-        <v>0</v>
+        <v>35709551237700.648</v>
       </c>
       <c r="G10" s="7">
         <f>BCEU_consumoBTU!I43*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E67</f>
-        <v>0</v>
+        <v>35810311822457.133</v>
       </c>
       <c r="H10" s="7">
         <f>BCEU_consumoBTU!J43*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E67</f>
-        <v>0</v>
+        <v>35895958319500.148</v>
       </c>
       <c r="I10" s="7">
         <f>BCEU_consumoBTU!K43*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E67</f>
-        <v>0</v>
+        <v>35996718904256.648</v>
       </c>
       <c r="J10" s="7">
         <f>BCEU_consumoBTU!L43*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E67</f>
-        <v>0</v>
+        <v>36092441459775.312</v>
       </c>
       <c r="K10" s="7">
         <f>BCEU_consumoBTU!M43*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E67</f>
-        <v>0</v>
+        <v>36193202044531.812</v>
       </c>
       <c r="L10" s="7">
         <f>BCEU_consumoBTU!N43*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E67</f>
-        <v>0</v>
+        <v>36288924600050.469</v>
       </c>
       <c r="M10" s="7">
         <f>BCEU_consumoBTU!O43*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E67</f>
-        <v>0</v>
+        <v>36384647155569.141</v>
       </c>
       <c r="N10" s="7">
         <f>BCEU_consumoBTU!P43*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E67</f>
-        <v>0</v>
+        <v>36374571097093.492</v>
       </c>
       <c r="O10" s="7">
         <f>BCEU_consumoBTU!Q43*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E67</f>
-        <v>0</v>
+        <v>36920189663549.883</v>
       </c>
       <c r="P10" s="7">
         <f>BCEU_consumoBTU!R43*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E67</f>
-        <v>0</v>
+        <v>37473992508503.133</v>
       </c>
       <c r="Q10" s="7">
         <f>BCEU_consumoBTU!S43*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E67</f>
-        <v>0</v>
+        <v>38036102396130.68</v>
       </c>
       <c r="R10" s="7">
         <f>BCEU_consumoBTU!T43*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E67</f>
-        <v>0</v>
+        <v>38606643932072.641</v>
       </c>
       <c r="S10" s="7">
         <f>BCEU_consumoBTU!U43*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E67</f>
-        <v>0</v>
+        <v>39185743591053.719</v>
       </c>
       <c r="T10" s="7">
         <f>BCEU_consumoBTU!V43*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E67</f>
-        <v>0</v>
+        <v>39773529744919.523</v>
       </c>
       <c r="U10" s="7">
         <f>BCEU_consumoBTU!W43*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E67</f>
-        <v>0</v>
+        <v>40370132691093.32</v>
       </c>
       <c r="V10" s="7">
         <f>BCEU_consumoBTU!X43*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E67</f>
-        <v>0</v>
+        <v>40975684681459.711</v>
       </c>
       <c r="W10" s="7">
         <f>BCEU_consumoBTU!Y43*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E67</f>
-        <v>0</v>
+        <v>41590319951681.609</v>
       </c>
       <c r="X10" s="7">
         <f>BCEU_consumoBTU!Z43*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E67</f>
-        <v>0</v>
+        <v>42214174750956.828</v>
       </c>
       <c r="Y10" s="7">
         <f>BCEU_consumoBTU!AA43*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E67</f>
-        <v>0</v>
+        <v>42847387372221.18</v>
       </c>
       <c r="Z10" s="7">
         <f>BCEU_consumoBTU!AB43*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E67</f>
-        <v>0</v>
+        <v>43490098182804.484</v>
       </c>
       <c r="AA10" s="7">
         <f>BCEU_consumoBTU!AC43*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E67</f>
-        <v>0</v>
+        <v>44142449655546.555</v>
       </c>
       <c r="AB10" s="7">
         <f>BCEU_consumoBTU!AD43*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E67</f>
-        <v>0</v>
+        <v>44804586400379.742</v>
       </c>
       <c r="AC10" s="7">
         <f>BCEU_consumoBTU!AE43*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E67</f>
-        <v>0</v>
+        <v>45476655196385.438</v>
       </c>
       <c r="AD10" s="7">
         <f>BCEU_consumoBTU!AF43*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E67</f>
-        <v>0</v>
+        <v>46158805024331.211</v>
       </c>
       <c r="AE10" s="7">
         <f>BCEU_consumoBTU!AG43*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E67</f>
-        <v>0</v>
+        <v>46851187099696.18</v>
       </c>
       <c r="AF10" s="7">
         <f>BCEU_consumoBTU!AH43*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E67</f>
-        <v>0</v>
+        <v>47553954906191.617</v>
       </c>
       <c r="AG10" s="7">
         <f>BCEU_consumoBTU!AI43*'BNE Fuel &amp; component splits'!$D$40*'BNE Fuel &amp; component splits'!$E67</f>
-        <v>0</v>
+        <v>48267264229784.484</v>
       </c>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.2">
@@ -34527,7 +34527,9 @@
   </sheetPr>
   <dimension ref="A3:AI48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -43348,7 +43350,7 @@
       <c r="R23" s="16" t="s">
         <v>250</v>
       </c>
-      <c r="S23" s="113">
+      <c r="S23" s="110">
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
@@ -43356,7 +43358,7 @@
       <c r="R24" s="16" t="s">
         <v>155</v>
       </c>
-      <c r="S24" s="114">
+      <c r="S24" s="111">
         <v>-5.0000000000000001E-3</v>
       </c>
     </row>
@@ -43367,7 +43369,7 @@
       <c r="R25" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="S25" s="114">
+      <c r="S25" s="111">
         <v>-5.0000000000000001E-3</v>
       </c>
     </row>
@@ -43752,7 +43754,7 @@
         <v>1.3511307458785089</v>
       </c>
       <c r="AK29" s="16">
-        <f t="shared" ref="G29:AK29" si="33">AK28/$F28</f>
+        <f t="shared" ref="AK29" si="33">AK28/$F28</f>
         <v>1.3713977070666865</v>
       </c>
     </row>
@@ -46611,17 +46613,25 @@
   </sheetPr>
   <dimension ref="A1:AF87"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="P53" zoomScale="125" workbookViewId="0">
+      <selection activeCell="U59" sqref="U59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="36.1640625" style="16" customWidth="1"/>
     <col min="2" max="2" width="18.83203125" style="16" customWidth="1"/>
-    <col min="3" max="8" width="10.83203125" style="16"/>
+    <col min="3" max="3" width="11.83203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="11" style="16" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.1640625" style="16" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="16"/>
+    <col min="10" max="15" width="11" style="16" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.83203125" style="16"/>
+    <col min="17" max="17" width="11" style="16" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.83203125" style="16"/>
+    <col min="19" max="19" width="11" style="16" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="10.83203125" style="16"/>
+    <col min="22" max="32" width="11" style="16" bestFit="1" customWidth="1"/>
+    <col min="33" max="16384" width="10.83203125" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -47852,75 +47862,75 @@
       <c r="J46" s="61"/>
       <c r="K46" s="61">
         <f t="shared" ref="K46:K56" si="4">X46/SUM(X$46:X$56)</f>
-        <v>1</v>
+        <v>0.06</v>
       </c>
       <c r="L46" s="61"/>
       <c r="M46" s="61">
         <f t="shared" ref="M46:O56" si="5">Z46/SUM(Z$46:Z$56)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N46" s="61">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O46" s="61">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P46" s="61"/>
       <c r="Q46" s="61">
         <f t="shared" ref="Q46:Q56" si="6">AD46/SUM(AD$46:AD$56)</f>
-        <v>1</v>
+        <v>0.06</v>
       </c>
       <c r="R46" s="61"/>
       <c r="S46" s="61">
         <f t="shared" ref="S46:S56" si="7">AF46/SUM(AF$46:AF$56)</f>
-        <v>0.76756058375992409</v>
+        <v>2.5411884351773464E-2</v>
       </c>
       <c r="T46" s="17"/>
       <c r="U46" s="17" t="s">
         <v>219</v>
       </c>
       <c r="V46" s="61">
-        <f>SUM(H6:H8)</f>
+        <f>H6</f>
         <v>0</v>
       </c>
       <c r="W46" s="61">
         <v>0</v>
       </c>
       <c r="X46" s="61">
-        <f>SUM(G6:G8)</f>
-        <v>31.563032</v>
+        <f>G6</f>
+        <v>1.8937819199999999</v>
       </c>
       <c r="Y46" s="61">
-        <f>SUM(F6:F8)</f>
+        <f>SUM(F6)</f>
         <v>0</v>
       </c>
       <c r="Z46" s="61">
-        <f>SUM(B6:B8)</f>
-        <v>2.7664840000000002</v>
+        <f>B6</f>
+        <v>0</v>
       </c>
       <c r="AA46" s="61">
-        <f>SUM(C6:C8)</f>
-        <v>259.31090699999999</v>
+        <f>SUM(C6)</f>
+        <v>0</v>
       </c>
       <c r="AB46" s="61">
-        <f>SUM(E6:E8)</f>
-        <v>1.1775230000000001</v>
+        <f>E6</f>
+        <v>0</v>
       </c>
       <c r="AC46" s="61">
         <v>0</v>
       </c>
       <c r="AD46" s="61">
-        <f>+SUM(D6:D8)</f>
-        <v>292.52786200000003</v>
+        <f>+SUM(D6)</f>
+        <v>17.551671720000002</v>
       </c>
       <c r="AE46" s="61">
         <v>0</v>
       </c>
       <c r="AF46" s="61">
         <f t="shared" ref="AF46:AF63" si="8">SUM(V46:AE46)</f>
-        <v>587.34580800000003</v>
+        <v>19.44545364</v>
       </c>
     </row>
     <row r="47" spans="1:32" x14ac:dyDescent="0.2">
@@ -48034,7 +48044,7 @@
       </c>
       <c r="B48" s="89">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0.06</v>
       </c>
       <c r="C48" s="100">
         <f t="shared" si="2"/>
@@ -48046,7 +48056,7 @@
       </c>
       <c r="E48" s="100">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.94000000000000006</v>
       </c>
       <c r="F48" s="89">
         <f t="shared" si="2"/>
@@ -48167,75 +48177,75 @@
       <c r="J49" s="61"/>
       <c r="K49" s="61">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.94000000000000006</v>
       </c>
       <c r="L49" s="61"/>
       <c r="M49" s="61">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N49" s="61">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O49" s="61">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P49" s="61"/>
       <c r="Q49" s="61">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.94</v>
       </c>
       <c r="R49" s="61"/>
       <c r="S49" s="61">
         <f t="shared" si="7"/>
-        <v>0.11621970812003787</v>
+        <v>0.85836840752818855</v>
       </c>
       <c r="T49" s="17"/>
       <c r="U49" s="17" t="s">
         <v>222</v>
       </c>
       <c r="V49" s="61">
-        <f>SUM(H12:H14)</f>
+        <f>SUM(H7:H8)+SUM(H12:H14)</f>
         <v>88.932599999999979</v>
       </c>
       <c r="W49" s="61">
         <v>0</v>
       </c>
       <c r="X49" s="61">
-        <f>SUM(G12:G14)</f>
-        <v>0</v>
+        <f>SUM(G7:G8)+SUM(G12:G14)</f>
+        <v>29.669250080000001</v>
       </c>
       <c r="Y49" s="61">
-        <f>SUM(F12:F14)</f>
+        <f>SUM(F7:F8)+SUM(F12:F14)</f>
         <v>0</v>
       </c>
       <c r="Z49" s="61">
-        <f>SUM(B12:B14)</f>
-        <v>0</v>
+        <f>SUM(B7:B8)+SUM(B12:B14)</f>
+        <v>2.7664840000000002</v>
       </c>
       <c r="AA49" s="61">
-        <f>SUM(C12:C14)</f>
-        <v>0</v>
+        <f>SUM(C7:C8)+SUM(C12:C14)</f>
+        <v>259.31090699999999</v>
       </c>
       <c r="AB49" s="61">
-        <f>SUM(E12:E12)</f>
-        <v>0</v>
+        <f>SUM(E7:E8)+SUM(E12:E12)</f>
+        <v>1.1775230000000001</v>
       </c>
       <c r="AC49" s="61">
         <v>0</v>
       </c>
       <c r="AD49" s="61">
-        <f>+SUM(D12:D14)</f>
-        <v>0</v>
+        <f>SUM(D7:D8)+SUM(D12:D14)</f>
+        <v>274.97619028000003</v>
       </c>
       <c r="AE49" s="61">
         <v>0</v>
       </c>
       <c r="AF49" s="61">
         <f t="shared" si="8"/>
-        <v>88.932599999999979</v>
+        <v>656.83295436000003</v>
       </c>
     </row>
     <row r="50" spans="1:32" x14ac:dyDescent="0.2">
@@ -48244,7 +48254,7 @@
       </c>
       <c r="B50" s="89">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C50" s="100">
         <f t="shared" si="2"/>
@@ -48256,7 +48266,7 @@
       </c>
       <c r="E50" s="100">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F50" s="89">
         <f t="shared" si="2"/>
@@ -48349,7 +48359,7 @@
       </c>
       <c r="B51" s="89">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C51" s="100">
         <f t="shared" si="2"/>
@@ -48361,7 +48371,7 @@
       </c>
       <c r="E51" s="100">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F51" s="89">
         <f t="shared" si="2"/>
@@ -48420,7 +48430,7 @@
       </c>
       <c r="B52" s="89">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C52" s="100">
         <f t="shared" si="2"/>
@@ -48432,7 +48442,7 @@
       </c>
       <c r="E52" s="100">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F52" s="89">
         <f t="shared" si="2"/>
@@ -48562,7 +48572,7 @@
       </c>
       <c r="B54" s="89">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0.06</v>
       </c>
       <c r="C54" s="100">
         <f t="shared" si="2"/>
@@ -48574,7 +48584,7 @@
       </c>
       <c r="E54" s="100">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.94</v>
       </c>
       <c r="F54" s="89">
         <f t="shared" si="2"/>
@@ -48925,7 +48935,7 @@
       <c r="J59" s="61"/>
       <c r="K59" s="61">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="L59" s="61">
         <f t="shared" si="10"/>
@@ -48933,60 +48943,60 @@
       </c>
       <c r="M59" s="61">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N59" s="61"/>
       <c r="O59" s="61"/>
       <c r="P59" s="61"/>
       <c r="Q59" s="61">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0.39999999999999997</v>
       </c>
       <c r="R59" s="61"/>
       <c r="S59" s="61">
         <f t="shared" si="10"/>
-        <v>0.50211048358681987</v>
+        <v>0.21037954928761174</v>
       </c>
       <c r="T59" s="17"/>
       <c r="U59" s="17" t="s">
         <v>219</v>
       </c>
       <c r="V59" s="61">
-        <f>SUM(H18:H20)</f>
+        <f>H18</f>
         <v>0</v>
       </c>
       <c r="W59" s="61">
         <v>0</v>
       </c>
       <c r="X59" s="61">
-        <f>SUM(G18:G20)</f>
-        <v>9.8046330000000008</v>
+        <f>G18</f>
+        <v>3.9218532000000006</v>
       </c>
       <c r="Y59" s="61">
-        <f>SUM(F18:F20)</f>
+        <f>F18</f>
         <v>3.721981</v>
       </c>
       <c r="Z59" s="61">
-        <f>SUM(B18:B20)</f>
-        <v>1.863747</v>
+        <f>B18</f>
+        <v>0</v>
       </c>
       <c r="AA59" s="61">
-        <f>SUM(C18:C20)</f>
+        <f>C18</f>
         <v>0</v>
       </c>
       <c r="AB59" s="61">
-        <f>SUM(E18:E20)</f>
+        <f>E18</f>
         <v>0</v>
       </c>
       <c r="AC59" s="61"/>
       <c r="AD59" s="61">
-        <f>+SUM(D18:D20)</f>
-        <v>62.948051999999997</v>
+        <f>D18</f>
+        <v>25.1792208</v>
       </c>
       <c r="AE59" s="61"/>
       <c r="AF59" s="61">
         <f t="shared" si="8"/>
-        <v>78.338413000000003</v>
+        <v>32.823054999999997</v>
       </c>
     </row>
     <row r="60" spans="1:32" x14ac:dyDescent="0.2">
@@ -49093,7 +49103,7 @@
       </c>
       <c r="B61" s="89">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="C61" s="89">
         <f t="shared" si="9"/>
@@ -49105,7 +49115,7 @@
       </c>
       <c r="E61" s="89">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="F61" s="89">
         <f t="shared" si="9"/>
@@ -49219,7 +49229,7 @@
       <c r="J62" s="61"/>
       <c r="K62" s="61">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="L62" s="61">
         <f t="shared" si="10"/>
@@ -49227,60 +49237,60 @@
       </c>
       <c r="M62" s="61">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N62" s="61"/>
       <c r="O62" s="61"/>
       <c r="P62" s="61"/>
       <c r="Q62" s="61">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="R62" s="61"/>
       <c r="S62" s="61">
         <f t="shared" si="10"/>
-        <v>6.9708331676223922E-2</v>
+        <v>0.36143926597543208</v>
       </c>
       <c r="T62" s="17"/>
       <c r="U62" s="17" t="s">
         <v>222</v>
       </c>
       <c r="V62" s="61">
-        <f>SUM(H21,H28)</f>
+        <f>SUM(H19:H21,H28)</f>
         <v>10.875773868300001</v>
       </c>
       <c r="W62" s="61">
         <v>0</v>
       </c>
       <c r="X62" s="61">
-        <f>SUM(G21,G28)</f>
-        <v>0</v>
+        <f>SUM(G19:G21,G28)</f>
+        <v>5.8827798000000007</v>
       </c>
       <c r="Y62" s="61">
-        <f>SUM(F21,F28)</f>
+        <f>SUM(F19:F21,F28)</f>
         <v>0</v>
       </c>
       <c r="Z62" s="61">
-        <f>SUM(B21,B28)</f>
-        <v>0</v>
+        <f>SUM(B19:B21,B28)</f>
+        <v>1.863747</v>
       </c>
       <c r="AA62" s="61">
-        <f>SUM(C21,C28)</f>
+        <f>SUM(C19:C21,C28)</f>
         <v>0</v>
       </c>
       <c r="AB62" s="61">
-        <f>SUM(E21,E28)</f>
+        <f>SUM(E19:E21,E28)</f>
         <v>0</v>
       </c>
       <c r="AC62" s="61"/>
       <c r="AD62" s="61">
-        <f>+SUM(D21,D28)</f>
-        <v>0</v>
+        <f>SUM(D19:D21,D28)</f>
+        <v>37.768831200000001</v>
       </c>
       <c r="AE62" s="61"/>
       <c r="AF62" s="61">
         <f t="shared" si="8"/>
-        <v>10.875773868300001</v>
+        <v>56.391131868300008</v>
       </c>
     </row>
     <row r="63" spans="1:32" x14ac:dyDescent="0.2">
@@ -49289,7 +49299,7 @@
       </c>
       <c r="B63" s="89">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C63" s="89">
         <f t="shared" si="9"/>
@@ -49301,7 +49311,7 @@
       </c>
       <c r="E63" s="89">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F63" s="89">
         <f t="shared" si="9"/>
@@ -49529,7 +49539,7 @@
       </c>
       <c r="B67" s="89">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0.39999999999999997</v>
       </c>
       <c r="C67" s="89">
         <f t="shared" si="9"/>
@@ -49541,7 +49551,7 @@
       </c>
       <c r="E67" s="89">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="F67" s="89">
         <f t="shared" si="9"/>
@@ -49556,18 +49566,6 @@
       <c r="P67" s="61"/>
       <c r="Q67" s="61"/>
       <c r="R67" s="61"/>
-      <c r="U67" s="17"/>
-      <c r="V67" s="61"/>
-      <c r="W67" s="17"/>
-      <c r="X67" s="61"/>
-      <c r="Y67" s="61"/>
-      <c r="Z67" s="61"/>
-      <c r="AA67" s="61"/>
-      <c r="AB67" s="61"/>
-      <c r="AC67" s="61"/>
-      <c r="AD67" s="61"/>
-      <c r="AE67" s="61"/>
-      <c r="AF67" s="17"/>
     </row>
     <row r="68" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A68" s="86" t="s">
@@ -49602,18 +49600,6 @@
       <c r="P68" s="61"/>
       <c r="Q68" s="61"/>
       <c r="R68" s="61"/>
-      <c r="U68" s="17"/>
-      <c r="V68" s="61"/>
-      <c r="W68" s="17"/>
-      <c r="X68" s="61"/>
-      <c r="Y68" s="61"/>
-      <c r="Z68" s="61"/>
-      <c r="AA68" s="61"/>
-      <c r="AB68" s="61"/>
-      <c r="AC68" s="61"/>
-      <c r="AD68" s="61"/>
-      <c r="AE68" s="61"/>
-      <c r="AF68" s="17"/>
     </row>
     <row r="72" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A72" s="16" t="s">

</xml_diff>